<commit_message>
Incoroporación del componente 'ClienteUpdate' funcional entre otros detalles
</commit_message>
<xml_diff>
--- a/Modelo Relacional.xlsx
+++ b/Modelo Relacional.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/68b2e1f1d6d74863/Escritorio/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/68b2e1f1d6d74863/Documentos/ProyectoPubligrafit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="223" documentId="13_ncr:1_{BDCD35AE-F78C-4CED-AA5E-A0B16D7A7DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CBA6BDE-2DCD-4B66-94B5-DD704A64DCE0}"/>
+  <xr:revisionPtr revIDLastSave="225" documentId="13_ncr:1_{BDCD35AE-F78C-4CED-AA5E-A0B16D7A7DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A778213B-95CA-467A-9B8E-31A2BD14CAC4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{8EFB6E32-D706-481C-9F09-EC1CB389C7EA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="56">
   <si>
     <t>Usuario</t>
   </si>
@@ -876,7 +876,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -889,7 +889,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1794,8 +1793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3481D12-1EFB-4FBB-BBF5-7EBB5A0DC5F7}">
   <dimension ref="A2:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2048,12 +2047,14 @@
       <c r="I18" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="M18" s="4" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C19" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G19" s="8"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">

</xml_diff>

<commit_message>
Corrección de módulo clientes e incorporación de módulo de ventas con validaciones y función de CRUD
</commit_message>
<xml_diff>
--- a/Modelo Relacional.xlsx
+++ b/Modelo Relacional.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/68b2e1f1d6d74863/Documentos/ProyectoPubligrafit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="225" documentId="13_ncr:1_{BDCD35AE-F78C-4CED-AA5E-A0B16D7A7DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A778213B-95CA-467A-9B8E-31A2BD14CAC4}"/>
+  <xr:revisionPtr revIDLastSave="264" documentId="13_ncr:1_{BDCD35AE-F78C-4CED-AA5E-A0B16D7A7DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3453F01D-6D87-4590-A732-7C2CDC8FF2F7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{8EFB6E32-D706-481C-9F09-EC1CB389C7EA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="62">
   <si>
     <t>Usuario</t>
   </si>
@@ -335,8 +335,43 @@
     <t>Detalle_Compra</t>
   </si>
   <si>
-    <r>
-      <t>Id_Compra</t>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Teléfono </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(varchar)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tipo_Comprobante </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(varchar)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Id_Categoría </t>
     </r>
     <r>
       <rPr>
@@ -351,11 +386,8 @@
     </r>
   </si>
   <si>
-    <t>Cliente</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Teléfono </t>
+    <r>
+      <t xml:space="preserve">Contraseña </t>
     </r>
     <r>
       <rPr>
@@ -371,7 +403,91 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Tipo_Comprobante </t>
+      <t xml:space="preserve">Estado </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(boolean)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Total </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(float)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Id_Detalle_Compra </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Iva </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(float</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Id_Permiso </t>
     </r>
     <r>
       <rPr>
@@ -387,7 +503,23 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Id_Categoría </t>
+      <t xml:space="preserve">Nombre_Rol </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(varchar)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Cantidad_Insumo </t>
     </r>
     <r>
       <rPr>
@@ -403,7 +535,119 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Iva </t>
+      <t xml:space="preserve">Imagen_Producto_Final </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(jpg, png, git)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Nombre_Producto </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(varchar)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Imagen </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(jpg, png, git)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Id_Detalle_Venta </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(int)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Documento </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(int)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Total </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(decimal)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fk_Id_Cliente </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(int)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Precio </t>
     </r>
     <r>
       <rPr>
@@ -419,7 +663,87 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Contraseña </t>
+      <t xml:space="preserve">Fk_Categoría </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(int)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fk_Venta </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(int)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fk_Producto </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(int)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Subtotal </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(float)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Id_Cliente </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(int)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tipo_Documento </t>
     </r>
     <r>
       <rPr>
@@ -435,23 +759,23 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Estado </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(boolean)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Total </t>
+      <t xml:space="preserve">Documento </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(varchar)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Precio_Final_Producto </t>
     </r>
     <r>
       <rPr>
@@ -467,18 +791,18 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Id_Detalle_Compra </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(int</t>
+      <t xml:space="preserve">Subtotal </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(float</t>
     </r>
     <r>
       <rPr>
@@ -493,65 +817,23 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Iva </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(float</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Id_Permiso </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(varchar)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Nombre_Rol </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(varchar)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Cantidad_Insumo </t>
+      <t xml:space="preserve">Precio_Insumo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(float)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fk_Insumo </t>
     </r>
     <r>
       <rPr>
@@ -567,55 +849,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Imagen_Producto_Final </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(jpg, png, git)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Nombre_Producto </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(varchar)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Imagen </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(jpg, png, git)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Stock </t>
+      <t xml:space="preserve">Fk_Rol </t>
     </r>
     <r>
       <rPr>
@@ -631,7 +865,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Id_Detalle_Venta </t>
+      <t>Fk_Compra</t>
     </r>
     <r>
       <rPr>
@@ -643,144 +877,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>(int)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Documento_Cliente </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(int)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Documento </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(int)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Total </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(decimal)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Precio </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(decimal)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Subtotal </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(decimal</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Precio_Insumo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(decimal)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Precio_Final_Producto </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(decimal)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Subtotal </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(decimal)</t>
     </r>
   </si>
 </sst>
@@ -1070,9 +1166,9 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
@@ -1093,8 +1189,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1343025" y="2190750"/>
-          <a:ext cx="1047750" cy="1400175"/>
+          <a:off x="1638300" y="2590800"/>
+          <a:ext cx="1038225" cy="1000125"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1793,13 +1889,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3481D12-1EFB-4FBB-BBF5-7EBB5A0DC5F7}">
   <dimension ref="A2:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" customWidth="1"/>
@@ -1808,7 +1904,7 @@
     <col min="7" max="7" width="31.7109375" customWidth="1"/>
     <col min="9" max="9" width="20.7109375" customWidth="1"/>
     <col min="11" max="11" width="26" customWidth="1"/>
-    <col min="13" max="13" width="17.42578125" customWidth="1"/>
+    <col min="13" max="13" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -1837,15 +1933,15 @@
         <v>23</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>22</v>
@@ -1856,36 +1952,44 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>36</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="C11" s="6" t="s">
         <v>5</v>
       </c>
@@ -1902,13 +2006,10 @@
         <v>7</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>6</v>
-      </c>
       <c r="C12" s="1" t="s">
         <v>27</v>
       </c>
@@ -1919,73 +2020,70 @@
         <v>14</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="K12" s="4" t="s">
         <v>26</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="C13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="K13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="M13" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="E14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="K14" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>15</v>
@@ -1994,83 +2092,92 @@
         <v>13</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="I16" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="E18" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="C19" s="6" t="s">
         <v>28</v>
       </c>
+      <c r="M19" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E20" s="7"/>
+      <c r="M20" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
       <c r="C21" s="1" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>8</v>
@@ -2081,12 +2188,12 @@
         <v>15</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>10</v>
@@ -2094,12 +2201,12 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C26" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrección módulo clientes y ventas
</commit_message>
<xml_diff>
--- a/Modelo Relacional.xlsx
+++ b/Modelo Relacional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/68b2e1f1d6d74863/Documentos/ProyectoPubligrafit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="264" documentId="13_ncr:1_{BDCD35AE-F78C-4CED-AA5E-A0B16D7A7DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3453F01D-6D87-4590-A732-7C2CDC8FF2F7}"/>
+  <xr:revisionPtr revIDLastSave="265" documentId="13_ncr:1_{BDCD35AE-F78C-4CED-AA5E-A0B16D7A7DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBF0827E-2C79-4FE0-A859-F29D43B1070D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{8EFB6E32-D706-481C-9F09-EC1CB389C7EA}"/>
   </bookViews>
@@ -355,7 +355,23 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Tipo_Comprobante </t>
+      <t xml:space="preserve">Id_Categoría </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(int)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Contraseña </t>
     </r>
     <r>
       <rPr>
@@ -371,7 +387,123 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Id_Categoría </t>
+      <t xml:space="preserve">Estado </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(boolean)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Total </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(float)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Id_Detalle_Compra </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Iva </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(float</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Id_Permiso </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(varchar)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Nombre_Rol </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(varchar)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Cantidad_Insumo </t>
     </r>
     <r>
       <rPr>
@@ -387,7 +519,23 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Contraseña </t>
+      <t xml:space="preserve">Imagen_Producto_Final </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(jpg, png, git)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Nombre_Producto </t>
     </r>
     <r>
       <rPr>
@@ -403,18 +551,50 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Estado </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(boolean)</t>
+      <t xml:space="preserve">Imagen </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(jpg, png, git)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Id_Detalle_Venta </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(int)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Documento </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(int)</t>
     </r>
   </si>
   <si>
@@ -430,23 +610,183 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>(decimal)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fk_Id_Cliente </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(int)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Precio </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>(float)</t>
     </r>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Id_Detalle_Compra </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(int</t>
+      <t xml:space="preserve">Fk_Categoría </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(int)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fk_Venta </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(int)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fk_Producto </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(int)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Subtotal </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(float)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Id_Cliente </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(int)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tipo_Documento </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(varchar)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Documento </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(varchar)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Precio_Final_Producto </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(float)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Subtotal </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(float</t>
     </r>
     <r>
       <rPr>
@@ -461,33 +801,71 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Iva </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(float</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Id_Permiso </t>
+      <t xml:space="preserve">Precio_Insumo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(float)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fk_Insumo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(int)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fk_Rol </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(int)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Fk_Compra</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(int)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Metodo_Pago </t>
     </r>
     <r>
       <rPr>
@@ -499,384 +877,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>(varchar)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Nombre_Rol </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(varchar)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Cantidad_Insumo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(int)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Imagen_Producto_Final </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(jpg, png, git)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Nombre_Producto </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(varchar)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Imagen </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(jpg, png, git)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Id_Detalle_Venta </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(int)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Documento </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(int)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Total </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(decimal)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Fk_Id_Cliente </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(int)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Precio </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(float)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Fk_Categoría </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(int)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Fk_Venta </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(int)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Fk_Producto </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(int)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Subtotal </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(float)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Id_Cliente </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(int)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Tipo_Documento </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(varchar)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Documento </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(varchar)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Precio_Final_Producto </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(float)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Subtotal </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(float</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Precio_Insumo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(float)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Fk_Insumo </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(int)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Fk_Rol </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(int)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Fk_Compra</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(int)</t>
     </r>
   </si>
 </sst>
@@ -1889,8 +1889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3481D12-1EFB-4FBB-BBF5-7EBB5A0DC5F7}">
   <dimension ref="A2:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1933,15 +1933,15 @@
         <v>23</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>22</v>
@@ -1952,18 +1952,18 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1983,12 +1983,12 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>5</v>
@@ -2020,13 +2020,13 @@
         <v>14</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K12" s="4" t="s">
         <v>26</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -2034,19 +2034,19 @@
         <v>10</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="K13" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -2054,22 +2054,22 @@
         <v>6</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -2080,10 +2080,10 @@
         <v>15</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>15</v>
@@ -2100,19 +2100,19 @@
         <v>17</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K16" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="M16" s="4" t="s">
         <v>19</v>
@@ -2123,13 +2123,13 @@
         <v>15</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M17" s="4" t="s">
         <v>30</v>
@@ -2143,7 +2143,7 @@
         <v>11</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M18" s="4" t="s">
         <v>18</v>
@@ -2151,7 +2151,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>28</v>
@@ -2162,22 +2162,22 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E20" s="7"/>
       <c r="M20" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
       <c r="C21" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>8</v>
@@ -2188,12 +2188,12 @@
         <v>15</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>10</v>
@@ -2201,12 +2201,12 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C26" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>